<commit_message>
factor(controller_factorise, model_factorise): Create classes of optional names of files and tabs involved in methods modifying the files
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_gather_columns_in_one - ref.xlsx
+++ b/fichiers_xls/test_gather_columns_in_one - ref.xlsx
@@ -9,8 +9,8 @@
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="tab_column_gathered_0" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="tab_column_gathered_1" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="tab_column_gathered_CDE" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="tab_column_gathered_GHI" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>

</xml_diff>